<commit_message>
Added to submission tracker and tweaked presentation notebook
</commit_message>
<xml_diff>
--- a/Blog/Capstone/submission_tracker.xlsx
+++ b/Blog/Capstone/submission_tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanbailey/Desktop/School/GA/Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanbailey/Desktop/Programming/Github/brendanbailey.github.io/Blog/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
   <si>
     <t>Model</t>
   </si>
@@ -299,13 +299,16 @@
   </si>
   <si>
     <t>model_20170524195902</t>
+  </si>
+  <si>
+    <t>model_20170525060947</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -341,6 +344,19 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -370,12 +386,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -638,11 +658,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="797861680"/>
-        <c:axId val="797863728"/>
+        <c:axId val="800351344"/>
+        <c:axId val="800406624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="797861680"/>
+        <c:axId val="800351344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,12 +718,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="797863728"/>
+        <c:crossAx val="800406624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="797863728"/>
+        <c:axId val="800406624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,6 +743,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -759,7 +780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="797861680"/>
+        <c:crossAx val="800351344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1662,11 +1683,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2838,6 +2859,34 @@
       <c r="H44" s="4">
         <v>0.88539999999999996</v>
       </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="7">
+        <v>42879</v>
+      </c>
+      <c r="E45" s="8">
+        <v>56</v>
+      </c>
+      <c r="F45" s="8">
+        <v>101</v>
+      </c>
+      <c r="G45">
+        <v>1.31856</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0.84209999999999996</v>
+      </c>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J44"/>

</xml_diff>

<commit_message>
Update site with Capstone Piece
</commit_message>
<xml_diff>
--- a/Blog/Capstone/submission_tracker.xlsx
+++ b/Blog/Capstone/submission_tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="20840" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="980" windowWidth="20840" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="92">
   <si>
     <t>Model</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>model_20170525060947</t>
+  </si>
+  <si>
+    <t>model_20170525194312.h5</t>
+  </si>
+  <si>
+    <t>Val loss estimated from graph</t>
   </si>
 </sst>
 </file>
@@ -658,11 +664,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="800351344"/>
-        <c:axId val="800406624"/>
+        <c:axId val="1705600512"/>
+        <c:axId val="1708479504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="800351344"/>
+        <c:axId val="1705600512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,6 +688,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -718,12 +725,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="800406624"/>
+        <c:crossAx val="1708479504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="800406624"/>
+        <c:axId val="1708479504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +787,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="800351344"/>
+        <c:crossAx val="1705600512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1683,11 +1690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2887,6 +2894,35 @@
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="2">
+        <v>42879</v>
+      </c>
+      <c r="E46" s="3">
+        <v>49</v>
+      </c>
+      <c r="F46" s="3">
+        <v>150</v>
+      </c>
+      <c r="G46">
+        <v>1.33521</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="J46" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J44"/>

</xml_diff>